<commit_message>
Added various new display scripts and added new system to accommodate plates with non-slat staples
</commit_message>
<xml_diff>
--- a/cargo_plates/sw_src004_polyAgridiron.xlsx
+++ b/cargo_plates/sw_src004_polyAgridiron.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stellawang/Documents/gitrepos/Crisscross-Design/cargo_plates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/cargo_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381423B7-BE65-E94B-8607-E90164E4D014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593BB293-A1F5-0B42-99F3-473869C55E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-58920" yWindow="-3600" windowWidth="26060" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Descriptions" sheetId="4" r:id="rId3"/>
     <sheet name="Extra Transfers" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="141">
   <si>
     <t>sw_src004</t>
   </si>
@@ -103,9 +103,111 @@
     <t>A</t>
   </si>
   <si>
+    <t>c0n0.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c0n2.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c0n4.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c2n0.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c2n2.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c2n4.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c4n0.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c4n2.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c4n4.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c6n0.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c6n2.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c6n4.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c8n0.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c8n2.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c8n4.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c10n0.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c10n2.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c10n4.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c12n0.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c12n2.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c12n4.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c14n0.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c14n2.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c14n4.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>polyA socketed gridiron staples</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
+    <t>c0n0.ext10.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c2n0.ext10.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c4n0.ext10.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c6n0.ext10.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c8n0.ext10.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c10n0.ext10.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c12n0.ext10.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>c14n0.ext10.10bpTH.A25</t>
+  </si>
+  <si>
+    <t>10nt CT extended socketed gridiron staples (left edge only)</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
@@ -224,6 +326,102 @@
   </si>
   <si>
     <t>from P3299_SW</t>
+  </si>
+  <si>
+    <t>GCCAGCAAAATGTTTATGTAGATGAAGGTATACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>ATAGCGATAGCGAGTTAGAGTCTGAGCAAAAACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>AGCCGGCGAACCTTACTGTTTCTTTACATAAACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>AGTAGCGACAGGTTTCTTGTTGTTCGCCATCCCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>CTCCGGCTTAGTGAGTATTACGAAGGTGTTATCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GCGTAACCACCCCAGGAGAACGAGGATATTGCCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GTTTGCCATCTGCAACACAGCAATAAAAATGCCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>CAAATATATTTTCATGCGTATTAACCAACAGTCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>TCCTCGTTAGATTAAGTTGGGTAACGCCAGGGCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GCCACCCTCAGCCTTCCTGTAGCCAGCTTTCACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>AGAATAAACACTTTGTTAAAATTCGCATTAAACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GTGTTTTTATACATATGTACCCCGGTTGATAACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GTCAGACGATTGCATAAAGCTAAATCGGTTGTCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>ACGCTCAACAGTCTACTAATAGTAGTAGCATTCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GTAATAACATCACCATTAGATACATTTCGCAACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>CCAGTAAGCGTAAAAATCAGGTCTTTACCCTGCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>AATAAGAGAATCAATACTGCGGAATCGTCATACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GCAACAGGAAAATAAAAACCAAAATAGCGAGACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GCCCGTATAAACGTAACAAAGCTGCTCATTCACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>ACGCGCCTGTTCGGTGTACAGACCAGGCGCATCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GTCACACGACCCTCCATGTTACTTAGCCGGAACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>AAGAGAAGGATGCCCACGCATAACCGATATATCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>AATAATCGGCTGTATCGGTTTATCAGCTTGCTCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GACAATATTTTAAGGAACAACTAAAGGAATTGCACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GCCAGCAAAATGTTTATGTAGATGAAGGTATA TTCCTCTTCT CACAACTACC AAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>AGTAGCGACAGGTTTCTTGTTGTTCGCCATCC TTCCTCTTCT CACAACTACC AAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GTTTGCCATCTGCAACACAGCAATAAAAATGC TTCCTCTTCT CACAACTACC AAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GCCACCCTCAGCCTTCCTGTAGCCAGCTTTCA TTCCTCTTCT CACAACTACC AAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GTCAGACGATTGCATAAAGCTAAATCGGTTGT TTCCTCTTCT CACAACTACC AAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>CCAGTAAGCGTAAAAATCAGGTCTTTACCCTG TTCCTCTTCT CACAACTACC AAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>GCCCGTATAAACGTAACAAAGCTGCTCATTCA TTCCTCTTCT CACAACTACC AAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>AAGAGAAGGATGCCCACGCATAACCGATATAT TTCCTCTTCT CACAACTACC AAAAAAAAAAAAAAAAAAAAAAAAA</t>
   </si>
   <si>
     <t>CTTGAAAACATAGATGATGAAACAAAACAAA TT CTCCTCAATC ACTATTCCTATTATAACTATACTT</t>
@@ -524,7 +722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -557,6 +755,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1736,7 +1937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1748,8 +1951,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
-        <v>74</v>
+      <c r="A1" s="34" t="s">
+        <v>140</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1829,71 +2032,139 @@
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="23"/>
+      <c r="B2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="30.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="22"/>
+        <v>51</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
+      <c r="E3" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
+      <c r="H3" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
+      <c r="K3" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="L3" s="21"/>
       <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
+      <c r="N3" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
-      <c r="Q3" s="22"/>
+      <c r="Q3" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="R3" s="21"/>
       <c r="S3" s="21"/>
-      <c r="T3" s="22"/>
+      <c r="T3" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
-      <c r="W3" s="22"/>
+      <c r="W3" s="22" t="s">
+        <v>59</v>
+      </c>
       <c r="X3" s="21"/>
       <c r="Y3" s="21"/>
-      <c r="Z3" s="22"/>
+      <c r="Z3" s="22" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>137</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -1917,13 +2188,11 @@
       <c r="W4" s="20"/>
       <c r="X4" s="20"/>
       <c r="Y4" s="20"/>
-      <c r="Z4" s="27" t="s">
-        <v>69</v>
-      </c>
+      <c r="Z4" s="24"/>
     </row>
     <row r="5" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -1953,7 +2222,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1983,7 +2252,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -2013,7 +2282,7 @@
     </row>
     <row r="8" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -2043,7 +2312,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -2073,7 +2342,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2103,7 +2372,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -2133,7 +2402,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -2163,7 +2432,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -2193,7 +2462,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -2223,7 +2492,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -2253,7 +2522,7 @@
     </row>
     <row r="16" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -2283,7 +2552,7 @@
     </row>
     <row r="17" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -2342,8 +2611,8 @@
   </sheetPr>
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView showGridLines="0" zoomScale="137" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2437,71 +2706,139 @@
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="7"/>
+      <c r="B2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="30.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="8"/>
+      <c r="H3" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="8"/>
+      <c r="K3" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
-      <c r="N3" s="8"/>
+      <c r="N3" s="8" t="s">
+        <v>129</v>
+      </c>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
-      <c r="Q3" s="8"/>
+      <c r="Q3" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="R3" s="9"/>
       <c r="S3" s="9"/>
-      <c r="T3" s="8"/>
+      <c r="T3" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
-      <c r="W3" s="8"/>
+      <c r="W3" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="X3" s="9"/>
       <c r="Y3" s="9"/>
-      <c r="Z3" s="10"/>
+      <c r="Z3" s="10" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>68</v>
+        <v>61</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>134</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -2525,13 +2862,13 @@
       <c r="W4" s="11"/>
       <c r="X4" s="11"/>
       <c r="Y4" s="11"/>
-      <c r="Z4" s="27" t="s">
-        <v>69</v>
+      <c r="Z4" s="28" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="11"/>
@@ -2561,7 +2898,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="11"/>
@@ -2591,7 +2928,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="11"/>
@@ -2621,7 +2958,7 @@
     </row>
     <row r="8" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="11"/>
@@ -2651,7 +2988,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="11"/>
@@ -2681,7 +3018,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="11"/>
@@ -2711,7 +3048,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -2741,7 +3078,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -2771,7 +3108,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -2801,7 +3138,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -2831,7 +3168,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -2861,7 +3198,7 @@
     </row>
     <row r="16" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -2891,7 +3228,7 @@
     </row>
     <row r="17" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -3072,319 +3409,383 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0930C350-316C-EA4B-A0EA-75FB866EE6DB}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Y3"/>
+    <sheetView topLeftCell="I1" zoomScale="107" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="28"/>
+    <col min="1" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="P2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="S2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="T2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="V2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="X2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y2" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="31"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="29"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="30"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="29" t="s">
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>40</v>
+      <c r="A17" s="29" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3397,7 +3798,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection sqref="A1:Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3479,84 +3880,84 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>

</xml_diff>